<commit_message>
Add opus big simple adapt wce results
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -558,45 +558,48 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,9 +619,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -636,6 +636,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1215,7 +1219,7 @@
       <c r="A8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="54" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="11">
@@ -1256,7 +1260,7 @@
       <c r="A9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="11">
         <v>42.523899999999998</v>
       </c>
@@ -1295,7 +1299,7 @@
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="12">
         <v>42.845599999999997</v>
       </c>
@@ -1375,7 +1379,7 @@
       <c r="A12" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="56" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="34">
@@ -1416,7 +1420,7 @@
       <c r="A13" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="34">
         <v>42.744900000000001</v>
       </c>
@@ -1455,7 +1459,7 @@
       <c r="A14" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="57"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="20">
         <v>42.728999999999999</v>
       </c>
@@ -1525,21 +1529,21 @@
       <c r="M16" s="33"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
@@ -1599,7 +1603,7 @@
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="1">
@@ -1640,7 +1644,7 @@
       <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="3">
         <v>36.130000000000003</v>
       </c>
@@ -1660,10 +1664,10 @@
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="3">
         <v>35.5</v>
       </c>
@@ -1681,8 +1685,8 @@
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="3">
         <v>35.409999999999997</v>
       </c>
@@ -1700,8 +1704,8 @@
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="3">
         <v>35.18</v>
       </c>
@@ -1719,8 +1723,8 @@
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="3">
         <v>31.63</v>
       </c>
@@ -1758,7 +1762,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2068,7 +2072,7 @@
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="54" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="16">
@@ -2109,7 +2113,7 @@
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="16">
         <v>43.3155</v>
       </c>
@@ -2148,7 +2152,7 @@
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="17">
         <v>43.175699999999999</v>
       </c>
@@ -2228,7 +2232,7 @@
       <c r="A12" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="59" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="30">
@@ -2269,7 +2273,7 @@
       <c r="A13" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="59"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="30">
         <v>42.972000000000001</v>
       </c>
@@ -2308,7 +2312,7 @@
       <c r="A14" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="60"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="31">
         <v>43.414900000000003</v>
       </c>
@@ -2452,7 +2456,7 @@
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="1">
@@ -2493,7 +2497,7 @@
       <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="3">
         <v>36.130000000000003</v>
       </c>
@@ -2513,10 +2517,10 @@
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="3">
         <v>35.5</v>
       </c>
@@ -2534,8 +2538,8 @@
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="3">
         <v>35.409999999999997</v>
       </c>
@@ -2553,8 +2557,8 @@
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="3">
         <v>35.18</v>
       </c>
@@ -2572,8 +2576,8 @@
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="3">
         <v>31.63</v>
       </c>
@@ -3020,7 +3024,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1">
@@ -3061,7 +3065,7 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="3">
         <v>36.130000000000003</v>
       </c>
@@ -3081,10 +3085,10 @@
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="3">
         <v>35.5</v>
       </c>
@@ -3102,8 +3106,8 @@
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="3">
         <v>35.409999999999997</v>
       </c>
@@ -3121,8 +3125,8 @@
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="3">
         <v>35.18</v>
       </c>
@@ -3140,8 +3144,8 @@
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="42"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="3">
         <v>31.63</v>
       </c>
@@ -3176,11 +3180,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3413,27 +3418,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3458,9 +3453,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finalise opus-big simple wce hyp search
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2101" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA87ABA-429C-4E84-BDBB-4C01F2B1D76F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="20580" windowHeight="12240" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test" sheetId="2" r:id="rId1"/>
@@ -1762,7 +1762,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3180,12 +3180,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3418,17 +3417,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3453,18 +3462,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add opus-big AoN wce results
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2101" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA87ABA-429C-4E84-BDBB-4C01F2B1D76F}"/>
+  <xr:revisionPtr revIDLastSave="2146" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09445E1B-FDEE-4AAF-B49E-6B21254A47F5}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="20580" windowHeight="12240" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="61">
   <si>
     <t>Validation BLEU</t>
   </si>
@@ -178,15 +178,6 @@
     <t>WCE-Random</t>
   </si>
   <si>
-    <t>0.75 train sample, full glossary, weight 1.25</t>
-  </si>
-  <si>
-    <t>0.1 train sample, full glossary, weight 1.25</t>
-  </si>
-  <si>
-    <t>0.25 train sample, full glossary, weight 1.5</t>
-  </si>
-  <si>
     <t>0.25 train sample, full glossary, upper weight 1.5, bands 6</t>
   </si>
   <si>
@@ -212,6 +203,24 @@
   </si>
   <si>
     <t>Simple Adaptive LSP WCE</t>
+  </si>
+  <si>
+    <t>1.0 train sampled glossary, 5 bands, weight 1.75</t>
+  </si>
+  <si>
+    <t>0.75 train sampled glossary, weight 1.25</t>
+  </si>
+  <si>
+    <t>0.1 train sampled glossary, weight 1.25</t>
+  </si>
+  <si>
+    <t>1.0 train sampled glossary, proportion 0.6, weight 1.5</t>
+  </si>
+  <si>
+    <t>1.0 train sampled glossary, bands 5, weight 1.25</t>
+  </si>
+  <si>
+    <t>0.25 train sampled glossary, weight 1.5</t>
   </si>
 </sst>
 </file>
@@ -908,8 +917,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C7" s="10">
         <v>43.001100000000001</v>
@@ -1220,7 +1229,7 @@
         <v>40</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" s="11">
         <v>42.563800000000001</v>
@@ -1339,7 +1348,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C11" s="21">
         <v>42.997799999999998</v>
@@ -1380,7 +1389,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12" s="34">
         <v>42.973199999999999</v>
@@ -1496,7 +1505,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
@@ -1513,41 +1522,89 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
+        <v>50</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="34">
+        <v>42.950499999999998</v>
+      </c>
+      <c r="D16" s="33">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="E16" s="33">
+        <v>52.65</v>
+      </c>
+      <c r="F16" s="33">
+        <v>69.540000000000006</v>
+      </c>
+      <c r="G16" s="33">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0.68620000000000003</v>
+      </c>
+      <c r="I16" s="33">
+        <v>960</v>
+      </c>
+      <c r="J16" s="33">
+        <v>0.68979999999999997</v>
+      </c>
+      <c r="K16" s="33">
+        <v>965</v>
+      </c>
+      <c r="L16" s="33">
+        <v>0.74909999999999999</v>
+      </c>
+      <c r="M16" s="33">
+        <v>1048</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
+        <v>51</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="40">
+        <v>43.082599999999999</v>
+      </c>
+      <c r="D17" s="41">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="E17" s="41">
+        <v>52.72</v>
+      </c>
+      <c r="F17" s="41">
+        <v>69.44</v>
+      </c>
+      <c r="G17" s="41">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H17" s="41">
+        <v>0.68189999999999995</v>
+      </c>
+      <c r="I17" s="41">
+        <v>954</v>
+      </c>
+      <c r="J17" s="41">
+        <v>0.68479999999999996</v>
+      </c>
+      <c r="K17" s="41">
+        <v>958</v>
+      </c>
+      <c r="L17" s="41">
+        <v>0.74619999999999997</v>
+      </c>
+      <c r="M17" s="41">
+        <v>1044</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -1564,7 +1621,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
@@ -1581,7 +1638,7 @@
     </row>
     <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -1761,8 +1818,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,7 +2089,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1">
         <v>43.105200000000004</v>
@@ -2073,7 +2130,7 @@
         <v>40</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" s="16">
         <v>43.083300000000001</v>
@@ -2192,7 +2249,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C11" s="22">
         <v>43.5535</v>
@@ -2233,7 +2290,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="30">
         <v>42.999899999999997</v>
@@ -2349,7 +2406,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" s="39"/>
       <c r="C15" s="22"/>
@@ -2366,24 +2423,48 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
+        <v>50</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="30">
+        <v>43.872199999999999</v>
+      </c>
+      <c r="D16" s="30">
+        <v>34.24</v>
+      </c>
+      <c r="E16" s="30">
+        <v>53.31</v>
+      </c>
+      <c r="F16" s="30">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="G16" s="30">
+        <v>0.51749999999999996</v>
+      </c>
+      <c r="H16" s="30">
+        <v>0.74409999999999998</v>
+      </c>
+      <c r="I16" s="30">
+        <v>1041</v>
+      </c>
+      <c r="J16" s="30">
+        <v>0.747</v>
+      </c>
+      <c r="K16" s="30">
+        <v>1045</v>
+      </c>
+      <c r="L16" s="30">
+        <v>0.747</v>
+      </c>
+      <c r="M16" s="30">
+        <v>1045</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" s="37"/>
       <c r="C17" s="30"/>
@@ -2400,7 +2481,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B18" s="37"/>
       <c r="C18" s="30"/>
@@ -2417,7 +2498,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" s="37"/>
       <c r="C19" s="30"/>
@@ -2434,7 +2515,7 @@
     </row>
     <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="31"/>

</xml_diff>

<commit_message>
Update opus-big fine lsp adapt wce
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2146" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09445E1B-FDEE-4AAF-B49E-6B21254A47F5}"/>
+  <xr:revisionPtr revIDLastSave="2148" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C47847FB-3223-4D7E-8D81-CB0B2230CC8D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
   <si>
     <t>Validation BLEU</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>0.25 train sampled glossary, weight 1.5</t>
+  </si>
+  <si>
+    <t>TUR-Exact</t>
   </si>
 </sst>
 </file>
@@ -917,8 +920,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>38</v>
@@ -1818,8 +1821,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1861,7 +1864,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>38</v>
@@ -3261,11 +3264,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3498,27 +3502,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3543,9 +3537,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
housekeeping and updating AoN and fine lsp results
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2148" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C47847FB-3223-4D7E-8D81-CB0B2230CC8D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test" sheetId="2" r:id="rId1"/>
@@ -648,10 +648,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,8 +916,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1821,8 +1817,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3264,12 +3260,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3502,17 +3497,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3537,18 +3542,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add updated prediction and result files
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2148" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C47847FB-3223-4D7E-8D81-CB0B2230CC8D}"/>
+  <xr:revisionPtr revIDLastSave="2161" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7CA5440-C510-4B36-9574-599F26950CDF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="65">
   <si>
     <t>Validation BLEU</t>
   </si>
@@ -224,6 +224,15 @@
   </si>
   <si>
     <t>TUR-Exact</t>
+  </si>
+  <si>
+    <t>Fine-Banded Unsampled Adaptive WCE</t>
+  </si>
+  <si>
+    <t>Simple Unsampled Adaptive WCE</t>
+  </si>
+  <si>
+    <t>All-or-Nothing Unsampled Adaptive WCE</t>
   </si>
 </sst>
 </file>
@@ -448,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,6 +581,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -914,10 +926,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8347FF-D187-4D6C-9C41-B96FB5C52911}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1227,7 +1239,7 @@
       <c r="A8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="55" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="11">
@@ -1268,7 +1280,7 @@
       <c r="A9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="43"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="11">
         <v>42.523899999999998</v>
       </c>
@@ -1307,7 +1319,7 @@
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="55"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="12">
         <v>42.845599999999997</v>
       </c>
@@ -1387,7 +1399,7 @@
       <c r="A12" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="57" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="34">
@@ -1428,7 +1440,7 @@
       <c r="A13" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="57"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="34">
         <v>42.744900000000001</v>
       </c>
@@ -1467,7 +1479,7 @@
       <c r="A14" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="20">
         <v>42.728999999999999</v>
       </c>
@@ -1520,290 +1532,341 @@
       <c r="M15" s="35"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="42"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B17" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C17" s="34">
         <v>42.950499999999998</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D17" s="33">
         <v>33.340000000000003</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E17" s="33">
         <v>52.65</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F17" s="33">
         <v>69.540000000000006</v>
       </c>
-      <c r="G16" s="33">
+      <c r="G17" s="33">
         <v>0.48480000000000001</v>
       </c>
-      <c r="H16" s="33">
+      <c r="H17" s="33">
         <v>0.68620000000000003</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I17" s="33">
         <v>960</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J17" s="33">
         <v>0.68979999999999997</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K17" s="33">
         <v>965</v>
       </c>
-      <c r="L16" s="33">
+      <c r="L17" s="33">
         <v>0.74909999999999999</v>
       </c>
-      <c r="M16" s="33">
+      <c r="M17" s="33">
         <v>1048</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="40">
-        <v>43.082599999999999</v>
-      </c>
-      <c r="D17" s="41">
-        <v>33.409999999999997</v>
-      </c>
-      <c r="E17" s="41">
-        <v>52.72</v>
-      </c>
-      <c r="F17" s="41">
-        <v>69.44</v>
-      </c>
-      <c r="G17" s="41">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="H17" s="41">
-        <v>0.68189999999999995</v>
-      </c>
-      <c r="I17" s="41">
-        <v>954</v>
-      </c>
-      <c r="J17" s="41">
-        <v>0.68479999999999996</v>
-      </c>
-      <c r="K17" s="41">
-        <v>958</v>
-      </c>
-      <c r="L17" s="41">
-        <v>0.74619999999999997</v>
-      </c>
-      <c r="M17" s="41">
-        <v>1044</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="40">
+        <v>43.082599999999999</v>
+      </c>
+      <c r="D19" s="41">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="E19" s="41">
+        <v>52.72</v>
+      </c>
+      <c r="F19" s="41">
+        <v>69.44</v>
+      </c>
+      <c r="G19" s="41">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H19" s="41">
+        <v>0.68189999999999995</v>
+      </c>
+      <c r="I19" s="41">
+        <v>954</v>
+      </c>
+      <c r="J19" s="41">
+        <v>0.68479999999999996</v>
+      </c>
+      <c r="K19" s="41">
+        <v>958</v>
+      </c>
+      <c r="L19" s="41">
+        <v>0.74619999999999997</v>
+      </c>
+      <c r="M19" s="41">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C24" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D24" s="1">
         <v>37.71</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E24" s="1">
         <v>55.04</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F24" s="1">
         <v>66.48</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G24" s="1">
         <v>0.5131</v>
       </c>
-      <c r="H21" s="26">
+      <c r="H24" s="26">
         <v>0.76480000000000004</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I24" s="1">
         <v>1070</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J24" s="1">
         <v>0.76700000000000002</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K24" s="1">
         <v>1073</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L24" s="1">
         <v>0.76700000000000002</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M24" s="1">
         <v>1073</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="3">
-        <v>36.130000000000003</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="3">
-        <v>35.5</v>
-      </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="3">
-        <v>35.409999999999997</v>
-      </c>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="44"/>
       <c r="D25" s="3">
-        <v>35.18</v>
-      </c>
-      <c r="E25" s="48"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="50"/>
+        <v>36.130000000000003</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="48"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="42"/>
+        <v>26</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="44"/>
       <c r="D26" s="3">
+        <v>35.5</v>
+      </c>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="51"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="3">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="51"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="3">
+        <v>35.18</v>
+      </c>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="51"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="3">
         <v>31.63</v>
       </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="53"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-    </row>
-    <row r="35" hidden="1" x14ac:dyDescent="0.3"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="54"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+    </row>
+    <row r="38" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="E22:M26"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="E25:M29"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B12:B14"/>
   </mergeCells>
@@ -1815,10 +1878,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2128,7 +2191,7 @@
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="55" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="16">
@@ -2169,7 +2232,7 @@
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="43"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="16">
         <v>43.3155</v>
       </c>
@@ -2208,7 +2271,7 @@
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="55"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="17">
         <v>43.175699999999999</v>
       </c>
@@ -2288,7 +2351,7 @@
       <c r="A12" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="60" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="30">
@@ -2329,7 +2392,7 @@
       <c r="A13" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="60"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="30">
         <v>42.972000000000001</v>
       </c>
@@ -2368,7 +2431,7 @@
       <c r="A14" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="61"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="31">
         <v>43.414900000000003</v>
       </c>
@@ -2421,66 +2484,66 @@
       <c r="M15" s="22"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="30">
-        <v>43.872199999999999</v>
-      </c>
-      <c r="D16" s="30">
-        <v>34.24</v>
-      </c>
-      <c r="E16" s="30">
-        <v>53.31</v>
-      </c>
-      <c r="F16" s="30">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="G16" s="30">
-        <v>0.51749999999999996</v>
-      </c>
-      <c r="H16" s="30">
-        <v>0.74409999999999998</v>
-      </c>
-      <c r="I16" s="30">
-        <v>1041</v>
-      </c>
-      <c r="J16" s="30">
-        <v>0.747</v>
-      </c>
-      <c r="K16" s="30">
-        <v>1045</v>
-      </c>
-      <c r="L16" s="30">
-        <v>0.747</v>
-      </c>
-      <c r="M16" s="30">
-        <v>1045</v>
-      </c>
+      <c r="A16" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
+        <v>50</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="30">
+        <v>43.872199999999999</v>
+      </c>
+      <c r="D17" s="30">
+        <v>34.24</v>
+      </c>
+      <c r="E17" s="30">
+        <v>53.31</v>
+      </c>
+      <c r="F17" s="30">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="G17" s="30">
+        <v>0.51749999999999996</v>
+      </c>
+      <c r="H17" s="30">
+        <v>0.74409999999999998</v>
+      </c>
+      <c r="I17" s="30">
+        <v>1041</v>
+      </c>
+      <c r="J17" s="30">
+        <v>0.747</v>
+      </c>
+      <c r="K17" s="30">
+        <v>1045</v>
+      </c>
+      <c r="L17" s="30">
+        <v>0.747</v>
+      </c>
+      <c r="M17" s="30">
+        <v>1045</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B18" s="37"/>
       <c r="C18" s="30"/>
@@ -2496,8 +2559,8 @@
       <c r="M18" s="30"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>54</v>
+      <c r="A19" s="41" t="s">
+        <v>51</v>
       </c>
       <c r="B19" s="37"/>
       <c r="C19" s="30"/>
@@ -2512,189 +2575,240 @@
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
     </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="37"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="B23" s="38"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C24" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D24" s="1">
         <v>37.71</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E24" s="1">
         <v>55.04</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F24" s="1">
         <v>66.48</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G24" s="1">
         <v>0.5131</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H24" s="1">
         <v>0.76480000000000004</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I24" s="1">
         <v>1070</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J24" s="1">
         <v>0.76700000000000002</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K24" s="1">
         <v>1073</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L24" s="1">
         <v>0.76700000000000002</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M24" s="1">
         <v>1073</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="3">
-        <v>36.130000000000003</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="3">
-        <v>35.5</v>
-      </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="3">
-        <v>35.409999999999997</v>
-      </c>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="44"/>
       <c r="D25" s="3">
-        <v>35.18</v>
-      </c>
-      <c r="E25" s="48"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="50"/>
+        <v>36.130000000000003</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="48"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="42"/>
+        <v>26</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="44"/>
       <c r="D26" s="3">
+        <v>35.5</v>
+      </c>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="51"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="3">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="51"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="3">
+        <v>35.18</v>
+      </c>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="51"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="3">
         <v>31.63</v>
       </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="53"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="54"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="E22:M26"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="E25:M29"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B12:B14"/>
   </mergeCells>
@@ -3104,7 +3218,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="44" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1">
@@ -3145,99 +3259,99 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="48"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="43"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="3">
         <v>35.5</v>
       </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="50"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="51"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="50"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="51"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="3">
         <v>35.18</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="50"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="51"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="44"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="3">
         <v>31.63</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="53"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="54"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
@@ -3268,6 +3382,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -3496,15 +3619,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
@@ -3523,6 +3637,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3539,12 +3661,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update supp data analysis
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2495" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0077F9BF-7416-410A-9866-20F527D43BAE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test" sheetId="2" r:id="rId1"/>
@@ -610,6 +610,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -644,9 +647,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -935,7 +935,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
@@ -1659,7 +1659,7 @@
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="41" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1">
@@ -1700,109 +1700,109 @@
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="41"/>
       <c r="D19" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="3">
         <v>35.5</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="48"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="3">
         <v>35.18</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="48"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="39"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="24">
         <f>MEDIAN(C7:C17)</f>
         <v>42.909500000000001</v>
@@ -1849,10 +1849,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="51"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="24">
         <f>MEDIAN(C9:C17)</f>
         <v>42.887900000000002</v>
@@ -1899,10 +1899,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="51"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="24">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>42.887900000000002</v>
@@ -1949,10 +1949,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="51"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="24">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>42.950499999999998</v>
@@ -1999,10 +1999,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="51"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="24">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>42.8215</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="51"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="24">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>42.772199999999998</v>
@@ -2063,7 +2063,7 @@
         <v>33.44</v>
       </c>
       <c r="E32" s="24">
-        <f t="shared" ref="D32:M32" si="5">MEDIAN(E10,E12,E14)</f>
+        <f t="shared" ref="E32:M32" si="5">MEDIAN(E10,E12,E14)</f>
         <v>52.65</v>
       </c>
       <c r="F32" s="24">
@@ -2100,10 +2100,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="51"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="24">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>42.950499999999998</v>
@@ -2150,10 +2150,10 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="51"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="24">
         <f>MEDIAN(C15:C17)</f>
         <v>42.8215</v>
@@ -2163,7 +2163,7 @@
         <v>33.409999999999997</v>
       </c>
       <c r="E34" s="24">
-        <f t="shared" ref="D34:M34" si="7">MEDIAN(E15:E17)</f>
+        <f t="shared" ref="E34:M34" si="7">MEDIAN(E15:E17)</f>
         <v>52.6</v>
       </c>
       <c r="F34" s="24">
@@ -2201,6 +2201,9 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="E19:M23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
@@ -2209,9 +2212,6 @@
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:M23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2223,7 +2223,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:M33"/>
     </sheetView>
   </sheetViews>
@@ -2947,7 +2947,7 @@
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="41" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1">
@@ -2988,109 +2988,109 @@
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="41"/>
       <c r="D19" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="3">
         <v>35.5</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="48"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="3">
         <v>35.18</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="48"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="39"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="24">
         <f>MEDIAN(C7:C17)</f>
         <v>43.5535</v>
@@ -3137,10 +3137,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="51"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="24">
         <f>MEDIAN(C9:C17)</f>
         <v>43.620199999999997</v>
@@ -3150,7 +3150,7 @@
         <v>33.9</v>
       </c>
       <c r="E27" s="24">
-        <f t="shared" ref="D27:M27" si="1">MEDIAN(E9:E17)</f>
+        <f t="shared" ref="E27:M27" si="1">MEDIAN(E9:E17)</f>
         <v>53.13</v>
       </c>
       <c r="F27" s="24">
@@ -3187,10 +3187,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="51"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="24">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>43.685600000000001</v>
@@ -3204,7 +3204,7 @@
         <v>53.23</v>
       </c>
       <c r="F28" s="24">
-        <f t="shared" ref="D28:M28" si="2">MEDIAN(F13,F14,F17)</f>
+        <f t="shared" ref="F28:M28" si="2">MEDIAN(F13,F14,F17)</f>
         <v>68.3</v>
       </c>
       <c r="G28" s="24">
@@ -3237,10 +3237,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="51"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="24">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>43.644100000000002</v>
@@ -3254,7 +3254,7 @@
         <v>53.13</v>
       </c>
       <c r="F29" s="24">
-        <f t="shared" ref="D29:M29" si="3">MEDIAN(F11,F12,F16)</f>
+        <f t="shared" ref="F29:M29" si="3">MEDIAN(F11,F12,F16)</f>
         <v>67.900000000000006</v>
       </c>
       <c r="G29" s="24">
@@ -3287,10 +3287,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="51"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="24">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>43.53</v>
@@ -3300,7 +3300,7 @@
         <v>33.85</v>
       </c>
       <c r="E30" s="24">
-        <f t="shared" ref="D30:M30" si="4">MEDIAN(E9,E10,E15)</f>
+        <f t="shared" ref="E30:M30" si="4">MEDIAN(E9,E10,E15)</f>
         <v>53.06</v>
       </c>
       <c r="F30" s="24">
@@ -3337,10 +3337,10 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="51"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="24">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>43.317</v>
@@ -3387,10 +3387,10 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="51"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="24">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>43.685600000000001</v>
@@ -3437,10 +3437,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="51"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="24">
         <f>MEDIAN(C15:C17)</f>
         <v>43.53</v>
@@ -3488,6 +3488,9 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="E19:M23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
@@ -3496,9 +3499,6 @@
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:M23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3906,7 +3906,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="41" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1">
@@ -3947,99 +3947,99 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="40"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="40"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="3">
         <v>35.5</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="48"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="48"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="3">
         <v>35.18</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="48"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="3">
         <v>31.63</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="50"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="51"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
@@ -4062,6 +4062,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -4290,38 +4307,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4344,9 +4333,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change adapt wce to fwce
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2495" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0077F9BF-7416-410A-9866-20F527D43BAE}"/>
+  <xr:revisionPtr revIDLastSave="2501" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34581960-9F73-4799-AA78-9C33C5131603}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="opus_base Test" sheetId="2" r:id="rId1"/>
-    <sheet name="opus_big Test " sheetId="4" r:id="rId2"/>
+    <sheet name="opus_base Test Results" sheetId="2" r:id="rId1"/>
+    <sheet name="opus_big Test Results " sheetId="4" r:id="rId2"/>
     <sheet name="M2M (Deprecated)" sheetId="6" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -160,24 +160,6 @@
     <t>M2M100_418M</t>
   </si>
   <si>
-    <t>Fine-Banded Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Simple Adaptive WCE</t>
-  </si>
-  <si>
-    <t>All-or-Nothing Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Fine-Banded LSP Adaptive WCE</t>
-  </si>
-  <si>
-    <t>All-or-Nothing LSP Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Simple Adaptive LSP WCE</t>
-  </si>
-  <si>
     <t>0.75 train sampled glossary, weight 1.25</t>
   </si>
   <si>
@@ -196,15 +178,6 @@
     <t>TUR-Exact</t>
   </si>
   <si>
-    <t>Fine-Banded Unsampled Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Simple Unsampled Adaptive WCE</t>
-  </si>
-  <si>
-    <t>All-or-Nothing Unsampled Adaptive WCE</t>
-  </si>
-  <si>
     <t>Unsampled glossary, proportion 0.2, weight 1.5</t>
   </si>
   <si>
@@ -250,25 +223,52 @@
     <t>Median across all WCE methods</t>
   </si>
   <si>
-    <t>Median for adaptive WCE</t>
-  </si>
-  <si>
-    <t>Median for Simple Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Median for All-or-Nothing Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Median for Fine-Banded Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Median for Unsampled Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Median for LSP Adaptive WCE</t>
-  </si>
-  <si>
-    <t>Median for Intersected Adaptive WCE</t>
+    <t>Simple LSP FWCE</t>
+  </si>
+  <si>
+    <t>Fine-Banded FWCE</t>
+  </si>
+  <si>
+    <t>Fine-Banded Unsampled FWCE</t>
+  </si>
+  <si>
+    <t>Simple FWCE</t>
+  </si>
+  <si>
+    <t>Simple Unsampled FWCE</t>
+  </si>
+  <si>
+    <t>All-or-Nothing FWCE</t>
+  </si>
+  <si>
+    <t>All-or-Nothing Unsampled FWCE</t>
+  </si>
+  <si>
+    <t>Fine-Banded LSP FWCE</t>
+  </si>
+  <si>
+    <t>All-or-Nothing LSP FWCE</t>
+  </si>
+  <si>
+    <t>Median for FWCE</t>
+  </si>
+  <si>
+    <t>Median for All-or-Nothing FWCE</t>
+  </si>
+  <si>
+    <t>Median for Simple FWCE</t>
+  </si>
+  <si>
+    <t>Median for Fine-Banded FWCE</t>
+  </si>
+  <si>
+    <t>Median for Unsampled FWCE</t>
+  </si>
+  <si>
+    <t>Median for Intersected FWCE</t>
+  </si>
+  <si>
+    <t>Median for LSP FWCE</t>
   </si>
 </sst>
 </file>
@@ -610,9 +610,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -647,6 +644,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -935,8 +935,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,7 +978,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>38</v>
@@ -1206,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" s="9">
         <v>43.001100000000001</v>
@@ -1247,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C8" s="18">
         <v>42.997799999999998</v>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C9" s="32">
         <v>42.909500000000001</v>
@@ -1326,10 +1326,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C10" s="32">
         <v>42.772199999999998</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C11" s="30">
         <v>42.950499999999998</v>
@@ -1408,10 +1408,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C12" s="36">
         <v>42.741199999999999</v>
@@ -1449,10 +1449,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>48</v>
       </c>
       <c r="C13" s="36">
         <v>43.082599999999999</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C14" s="36">
         <v>42.887900000000002</v>
@@ -1531,10 +1531,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C15" s="30">
         <v>42.8215</v>
@@ -1572,10 +1572,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C16" s="30">
         <v>43.1111</v>
@@ -1613,10 +1613,10 @@
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C17" s="17">
         <v>42.747900000000001</v>
@@ -1659,7 +1659,7 @@
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="40" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1">
@@ -1700,109 +1700,109 @@
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="45"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="41"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="3">
         <v>35.5</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="48"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="47"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="48"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="47"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="3">
         <v>35.18</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="48"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="41"/>
       <c r="D23" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="51"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="40"/>
+      <c r="A26" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="39"/>
       <c r="C26" s="24">
         <f>MEDIAN(C7:C17)</f>
         <v>42.909500000000001</v>
@@ -1849,10 +1849,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="39"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="24">
         <f>MEDIAN(C9:C17)</f>
         <v>42.887900000000002</v>
@@ -1899,10 +1899,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="39"/>
+      <c r="A28" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="51"/>
       <c r="C28" s="24">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>42.887900000000002</v>
@@ -1949,10 +1949,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="39"/>
+      <c r="A29" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="51"/>
       <c r="C29" s="24">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>42.950499999999998</v>
@@ -1999,10 +1999,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="39"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="24">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>42.8215</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="24">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>42.772199999999998</v>
@@ -2100,10 +2100,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="39"/>
+      <c r="A33" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="51"/>
       <c r="C33" s="24">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>42.950499999999998</v>
@@ -2150,10 +2150,10 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="39"/>
+      <c r="A34" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="51"/>
       <c r="C34" s="24">
         <f>MEDIAN(C15:C17)</f>
         <v>42.8215</v>
@@ -2201,17 +2201,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:M23"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="E19:M23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2223,8 +2223,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:M33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2266,7 +2266,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>38</v>
@@ -2494,7 +2494,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>43.105200000000004</v>
@@ -2535,7 +2535,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C8" s="19">
         <v>43.5535</v>
@@ -2573,10 +2573,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C9" s="19">
         <v>43.620199999999997</v>
@@ -2614,10 +2614,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C10" s="19">
         <v>43.218000000000004</v>
@@ -2655,10 +2655,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C11" s="26">
         <v>43.872199999999999</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C12" s="26">
         <v>43.644100000000002</v>
@@ -2737,10 +2737,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C13" s="26">
         <v>43.685600000000001</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="33" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>63</v>
       </c>
       <c r="C14" s="26">
         <v>43.317</v>
@@ -2819,10 +2819,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C15" s="26">
         <v>43.53</v>
@@ -2860,10 +2860,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C16" s="26">
         <v>43.3065</v>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C17" s="27">
         <v>43.733899999999998</v>
@@ -2947,7 +2947,7 @@
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="40" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1">
@@ -2988,109 +2988,109 @@
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="45"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="41"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="3">
         <v>35.5</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="48"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="47"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="48"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="47"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="3">
         <v>35.18</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="48"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="41"/>
       <c r="D23" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="51"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="40"/>
+      <c r="A26" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="39"/>
       <c r="C26" s="24">
         <f>MEDIAN(C7:C17)</f>
         <v>43.5535</v>
@@ -3137,10 +3137,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="39"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="24">
         <f>MEDIAN(C9:C17)</f>
         <v>43.620199999999997</v>
@@ -3187,10 +3187,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="39"/>
+      <c r="A28" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="51"/>
       <c r="C28" s="24">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>43.685600000000001</v>
@@ -3237,10 +3237,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="39"/>
+      <c r="A29" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="51"/>
       <c r="C29" s="24">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>43.644100000000002</v>
@@ -3287,10 +3287,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="39"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="24">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>43.53</v>
@@ -3337,10 +3337,10 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="39"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="24">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>43.317</v>
@@ -3387,10 +3387,10 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="39"/>
+      <c r="A32" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="51"/>
       <c r="C32" s="24">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>43.685600000000001</v>
@@ -3437,10 +3437,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="39"/>
+      <c r="A33" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="51"/>
       <c r="C33" s="24">
         <f>MEDIAN(C15:C17)</f>
         <v>43.53</v>
@@ -3488,17 +3488,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:M23"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="E19:M23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3906,7 +3906,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="40" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1">
@@ -3947,99 +3947,99 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="45"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="44"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="3">
         <v>35.5</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="48"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="47"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="48"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="47"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="3">
         <v>35.18</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="48"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="47"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="42"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="3">
         <v>31.63</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="51"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="50"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
@@ -4062,23 +4062,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -4307,10 +4290,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4333,20 +4344,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement concept detection using ontologies
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2501" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34581960-9F73-4799-AA78-9C33C5131603}"/>
+  <xr:revisionPtr revIDLastSave="2546" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D27AF67D-310C-4197-A324-BC84E971D6E8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test Results" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="80">
   <si>
     <t>Validation BLEU</t>
   </si>
@@ -175,9 +175,6 @@
     <t>0.25 train sampled glossary, weight 1.5</t>
   </si>
   <si>
-    <t>TUR-Exact</t>
-  </si>
-  <si>
     <t>Unsampled glossary, proportion 0.2, weight 1.5</t>
   </si>
   <si>
@@ -269,6 +266,18 @@
   </si>
   <si>
     <t>Median for LSP FWCE</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Annotated Concepts</t>
   </si>
 </sst>
 </file>
@@ -301,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +326,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,12 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,6 +619,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -645,7 +657,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -933,10 +954,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8347FF-D187-4D6C-9C41-B96FB5C52911}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,15 +968,13 @@
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="6" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
     <col min="9" max="9" width="17.88671875" customWidth="1"/>
     <col min="10" max="10" width="16.21875" customWidth="1"/>
     <col min="11" max="11" width="17.77734375" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -978,25 +997,19 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1018,26 +1031,20 @@
       <c r="G2" s="7">
         <v>0.48980000000000001</v>
       </c>
-      <c r="H2" s="22">
-        <v>0.72270000000000001</v>
+      <c r="H2" s="53">
+        <v>2116</v>
       </c>
       <c r="I2" s="11">
-        <v>1011</v>
+        <v>0.52629999999999999</v>
       </c>
       <c r="J2" s="11">
-        <v>0.72550000000000003</v>
+        <v>0.55810000000000004</v>
       </c>
       <c r="K2" s="11">
-        <v>1015</v>
-      </c>
-      <c r="L2" s="11">
-        <v>0.72550000000000003</v>
-      </c>
-      <c r="M2" s="11">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.54169999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1060,25 +1067,19 @@
         <v>0.4894</v>
       </c>
       <c r="H3" s="12">
-        <v>0.68620000000000003</v>
+        <v>2002</v>
       </c>
       <c r="I3" s="12">
-        <v>960</v>
+        <v>0.50670000000000004</v>
       </c>
       <c r="J3" s="12">
-        <v>0.68910000000000005</v>
+        <v>0.56789999999999996</v>
       </c>
       <c r="K3" s="12">
-        <v>964</v>
-      </c>
-      <c r="L3" s="12">
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="M3" s="12">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.53559999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1100,26 +1101,12 @@
       <c r="G4" s="8">
         <v>0.4723</v>
       </c>
-      <c r="H4" s="13">
-        <v>0.67410000000000003</v>
-      </c>
-      <c r="I4" s="13">
-        <v>943</v>
-      </c>
-      <c r="J4" s="13">
-        <v>0.67759999999999998</v>
-      </c>
-      <c r="K4" s="13">
-        <v>948</v>
-      </c>
-      <c r="L4" s="13">
-        <v>0.74409999999999998</v>
-      </c>
-      <c r="M4" s="13">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1141,26 +1128,12 @@
       <c r="G5" s="8">
         <v>0.4834</v>
       </c>
-      <c r="H5" s="13">
-        <v>0.67479999999999996</v>
-      </c>
-      <c r="I5" s="13">
-        <v>944</v>
-      </c>
-      <c r="J5" s="13">
-        <v>0.67759999999999998</v>
-      </c>
-      <c r="K5" s="13">
-        <v>948</v>
-      </c>
-      <c r="L5" s="13">
-        <v>0.74339999999999995</v>
-      </c>
-      <c r="M5" s="13">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1170,38 +1143,24 @@
       <c r="C6" s="4">
         <v>42.606000000000002</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>33.090000000000003</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>52.29</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="23">
         <v>69.459999999999994</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="23">
         <v>0.49020000000000002</v>
       </c>
-      <c r="H6" s="14">
-        <v>0.67479999999999996</v>
-      </c>
-      <c r="I6" s="14">
-        <v>944</v>
-      </c>
-      <c r="J6" s="14">
-        <v>0.67689999999999995</v>
-      </c>
-      <c r="K6" s="14">
-        <v>947</v>
-      </c>
-      <c r="L6" s="14">
-        <v>0.73480000000000001</v>
-      </c>
-      <c r="M6" s="14">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1223,27 +1182,13 @@
       <c r="G7" s="11">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H7" s="28">
-        <v>0.6905</v>
-      </c>
-      <c r="I7" s="28">
-        <v>966</v>
-      </c>
-      <c r="J7" s="28">
-        <v>0.69410000000000005</v>
-      </c>
-      <c r="K7" s="28">
-        <v>971</v>
-      </c>
-      <c r="L7" s="28">
-        <v>0.75270000000000004</v>
-      </c>
-      <c r="M7" s="28">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -1264,359 +1209,233 @@
       <c r="G8" s="19">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H8" s="19">
-        <v>0.68620000000000003</v>
-      </c>
-      <c r="I8" s="19">
-        <v>960</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0.68979999999999997</v>
-      </c>
-      <c r="K8" s="19">
-        <v>965</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="M8" s="19">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="30">
+        <v>42.909500000000001</v>
+      </c>
+      <c r="D9" s="29">
+        <v>33.369999999999997</v>
+      </c>
+      <c r="E9" s="29">
+        <v>52.64</v>
+      </c>
+      <c r="F9" s="29">
+        <v>69.61</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0.48470000000000002</v>
+      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B10" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="32">
-        <v>42.909500000000001</v>
-      </c>
-      <c r="D9" s="31">
-        <v>33.369999999999997</v>
-      </c>
-      <c r="E9" s="31">
-        <v>52.64</v>
-      </c>
-      <c r="F9" s="31">
-        <v>69.61</v>
-      </c>
-      <c r="G9" s="31">
-        <v>0.48470000000000002</v>
-      </c>
-      <c r="H9" s="31">
-        <v>0.68410000000000004</v>
-      </c>
-      <c r="I9" s="31">
-        <v>957</v>
-      </c>
-      <c r="J9" s="31">
-        <v>0.68759999999999999</v>
-      </c>
-      <c r="K9" s="31">
-        <v>962</v>
-      </c>
-      <c r="L9" s="31">
-        <v>0.74980000000000002</v>
-      </c>
-      <c r="M9" s="31">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="C10" s="30">
+        <v>42.772199999999998</v>
+      </c>
+      <c r="D10" s="29">
+        <v>33.44</v>
+      </c>
+      <c r="E10" s="29">
+        <v>52.62</v>
+      </c>
+      <c r="F10" s="29">
+        <v>69.569999999999993</v>
+      </c>
+      <c r="G10" s="29">
+        <v>0.48380000000000001</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B11" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="28">
+        <v>42.950499999999998</v>
+      </c>
+      <c r="D11" s="27">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="E11" s="27">
+        <v>52.65</v>
+      </c>
+      <c r="F11" s="27">
+        <v>69.540000000000006</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="34">
+        <v>42.741199999999999</v>
+      </c>
+      <c r="D12" s="35">
+        <v>34.130000000000003</v>
+      </c>
+      <c r="E12" s="35">
+        <v>53.07</v>
+      </c>
+      <c r="F12" s="35">
+        <v>68.489999999999995</v>
+      </c>
+      <c r="G12" s="35">
+        <v>0.48880000000000001</v>
+      </c>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="34">
+        <v>43.082599999999999</v>
+      </c>
+      <c r="D13" s="35">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="E13" s="35">
+        <v>52.72</v>
+      </c>
+      <c r="F13" s="35">
+        <v>69.44</v>
+      </c>
+      <c r="G13" s="35">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="34">
+        <v>42.887900000000002</v>
+      </c>
+      <c r="D14" s="35">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="E14" s="35">
+        <v>52.65</v>
+      </c>
+      <c r="F14" s="35">
+        <v>69.55</v>
+      </c>
+      <c r="G14" s="35">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="28">
+        <v>42.8215</v>
+      </c>
+      <c r="D15" s="27">
+        <v>33.76</v>
+      </c>
+      <c r="E15" s="27">
+        <v>52.76</v>
+      </c>
+      <c r="F15" s="27">
+        <v>69.42</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0.48509999999999998</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="28">
+        <v>43.1111</v>
+      </c>
+      <c r="D16" s="27">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="E16" s="27">
+        <v>52.6</v>
+      </c>
+      <c r="F16" s="27">
+        <v>69.790000000000006</v>
+      </c>
+      <c r="G16" s="27">
+        <v>0.48080000000000001</v>
+      </c>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="32">
-        <v>42.772199999999998</v>
-      </c>
-      <c r="D10" s="31">
-        <v>33.44</v>
-      </c>
-      <c r="E10" s="31">
-        <v>52.62</v>
-      </c>
-      <c r="F10" s="31">
-        <v>69.569999999999993</v>
-      </c>
-      <c r="G10" s="31">
-        <v>0.48380000000000001</v>
-      </c>
-      <c r="H10" s="31">
-        <v>0.68479999999999996</v>
-      </c>
-      <c r="I10" s="31">
-        <v>958</v>
-      </c>
-      <c r="J10" s="31">
-        <v>0.68830000000000002</v>
-      </c>
-      <c r="K10" s="31">
-        <v>963</v>
-      </c>
-      <c r="L10" s="31">
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M10" s="31">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="30">
-        <v>42.950499999999998</v>
-      </c>
-      <c r="D11" s="29">
-        <v>33.340000000000003</v>
-      </c>
-      <c r="E11" s="29">
-        <v>52.65</v>
-      </c>
-      <c r="F11" s="29">
-        <v>69.540000000000006</v>
-      </c>
-      <c r="G11" s="29">
-        <v>0.48480000000000001</v>
-      </c>
-      <c r="H11" s="29">
-        <v>0.68620000000000003</v>
-      </c>
-      <c r="I11" s="29">
-        <v>960</v>
-      </c>
-      <c r="J11" s="29">
-        <v>0.68979999999999997</v>
-      </c>
-      <c r="K11" s="29">
-        <v>965</v>
-      </c>
-      <c r="L11" s="29">
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M11" s="29">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="36">
-        <v>42.741199999999999</v>
-      </c>
-      <c r="D12" s="37">
-        <v>34.130000000000003</v>
-      </c>
-      <c r="E12" s="37">
-        <v>53.07</v>
-      </c>
-      <c r="F12" s="37">
-        <v>68.489999999999995</v>
-      </c>
-      <c r="G12" s="37">
-        <v>0.48880000000000001</v>
-      </c>
-      <c r="H12" s="37">
-        <v>0.6905</v>
-      </c>
-      <c r="I12" s="37">
-        <v>966</v>
-      </c>
-      <c r="J12" s="37">
-        <v>0.69340000000000002</v>
-      </c>
-      <c r="K12" s="37">
-        <v>970</v>
-      </c>
-      <c r="L12" s="37">
-        <v>0.74980000000000002</v>
-      </c>
-      <c r="M12" s="37">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="36">
-        <v>43.082599999999999</v>
-      </c>
-      <c r="D13" s="37">
-        <v>33.409999999999997</v>
-      </c>
-      <c r="E13" s="37">
-        <v>52.72</v>
-      </c>
-      <c r="F13" s="37">
-        <v>69.44</v>
-      </c>
-      <c r="G13" s="37">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="H13" s="37">
-        <v>0.68189999999999995</v>
-      </c>
-      <c r="I13" s="37">
-        <v>954</v>
-      </c>
-      <c r="J13" s="37">
-        <v>0.68479999999999996</v>
-      </c>
-      <c r="K13" s="37">
-        <v>958</v>
-      </c>
-      <c r="L13" s="37">
-        <v>0.74619999999999997</v>
-      </c>
-      <c r="M13" s="37">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="36">
-        <v>42.887900000000002</v>
-      </c>
-      <c r="D14" s="37">
-        <v>33.409999999999997</v>
-      </c>
-      <c r="E14" s="37">
-        <v>52.65</v>
-      </c>
-      <c r="F14" s="37">
-        <v>69.55</v>
-      </c>
-      <c r="G14" s="37">
-        <v>0.48549999999999999</v>
-      </c>
-      <c r="H14" s="37">
-        <v>0.68330000000000002</v>
-      </c>
-      <c r="I14" s="37">
-        <v>956</v>
-      </c>
-      <c r="J14" s="37">
-        <v>0.68689999999999996</v>
-      </c>
-      <c r="K14" s="37">
-        <v>961</v>
-      </c>
-      <c r="L14" s="37">
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="M14" s="37">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="30">
-        <v>42.8215</v>
-      </c>
-      <c r="D15" s="29">
-        <v>33.76</v>
-      </c>
-      <c r="E15" s="29">
-        <v>52.76</v>
-      </c>
-      <c r="F15" s="29">
-        <v>69.42</v>
-      </c>
-      <c r="G15" s="29">
-        <v>0.48509999999999998</v>
-      </c>
-      <c r="H15" s="29">
-        <v>0.6855</v>
-      </c>
-      <c r="I15" s="29">
-        <v>959</v>
-      </c>
-      <c r="J15" s="29">
-        <v>0.68910000000000005</v>
-      </c>
-      <c r="K15" s="29">
-        <v>964</v>
-      </c>
-      <c r="L15" s="29">
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M15" s="29">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="30">
-        <v>43.1111</v>
-      </c>
-      <c r="D16" s="29">
-        <v>33.409999999999997</v>
-      </c>
-      <c r="E16" s="29">
-        <v>52.6</v>
-      </c>
-      <c r="F16" s="29">
-        <v>69.790000000000006</v>
-      </c>
-      <c r="G16" s="29">
-        <v>0.48080000000000001</v>
-      </c>
-      <c r="H16" s="29">
-        <v>0.68759999999999999</v>
-      </c>
-      <c r="I16" s="29">
-        <v>962</v>
-      </c>
-      <c r="J16" s="29">
-        <v>0.6905</v>
-      </c>
-      <c r="K16" s="29">
-        <v>966</v>
-      </c>
-      <c r="L16" s="29">
-        <v>0.74980000000000002</v>
-      </c>
-      <c r="M16" s="29">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="C17" s="17">
         <v>42.747900000000001</v>
@@ -1633,33 +1452,19 @@
       <c r="G17" s="16">
         <v>0.48409999999999997</v>
       </c>
-      <c r="H17" s="16">
-        <v>0.68410000000000004</v>
-      </c>
-      <c r="I17" s="16">
-        <v>957</v>
-      </c>
-      <c r="J17" s="16">
-        <v>0.68759999999999999</v>
-      </c>
-      <c r="K17" s="16">
-        <v>962</v>
-      </c>
-      <c r="L17" s="16">
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M17" s="16">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1">
@@ -1674,544 +1479,456 @@
       <c r="G18" s="1">
         <v>0.5131</v>
       </c>
-      <c r="H18" s="23">
-        <v>0.76480000000000004</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1070</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1073</v>
-      </c>
-      <c r="L18" s="1">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="M18" s="1">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H18" s="52"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="3">
         <v>35.5</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="3">
         <v>35.18</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="24">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="22">
         <f>MEDIAN(C7:C17)</f>
         <v>42.909500000000001</v>
       </c>
-      <c r="D26" s="24">
-        <f t="shared" ref="D26:M26" si="0">MEDIAN(D7:D17)</f>
+      <c r="D26" s="22">
+        <f t="shared" ref="D26:K26" si="0">MEDIAN(D7:D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="22">
         <f t="shared" si="0"/>
         <v>52.65</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="22">
         <f t="shared" si="0"/>
         <v>69.55</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="22">
         <f t="shared" si="0"/>
         <v>0.48509999999999998</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>0.6855</v>
-      </c>
-      <c r="I26" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>959</v>
-      </c>
-      <c r="J26" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>0.68910000000000005</v>
-      </c>
-      <c r="K26" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>964</v>
-      </c>
-      <c r="L26" s="24">
-        <f t="shared" si="0"/>
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M26" s="24">
-        <f t="shared" si="0"/>
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="22">
         <f>MEDIAN(C9:C17)</f>
         <v>42.887900000000002</v>
       </c>
-      <c r="D27" s="24">
-        <f t="shared" ref="D27:M27" si="1">MEDIAN(D9:D17)</f>
+      <c r="D27" s="22">
+        <f t="shared" ref="D27:K27" si="1">MEDIAN(D9:D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="22">
         <f t="shared" si="1"/>
         <v>52.65</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="22">
         <f t="shared" si="1"/>
         <v>69.540000000000006</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="22">
         <f t="shared" si="1"/>
         <v>0.48480000000000001</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>0.68479999999999996</v>
-      </c>
-      <c r="I27" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>958</v>
-      </c>
-      <c r="J27" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>0.68830000000000002</v>
-      </c>
-      <c r="K27" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>963</v>
-      </c>
-      <c r="L27" s="24">
-        <f t="shared" si="1"/>
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M27" s="24">
-        <f t="shared" si="1"/>
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="22">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>42.887900000000002</v>
       </c>
-      <c r="D28" s="24">
-        <f t="shared" ref="D28:M28" si="2">MEDIAN(D13,D14,D17)</f>
+      <c r="D28" s="22">
+        <f t="shared" ref="D28:K28" si="2">MEDIAN(D13,D14,D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="22">
         <f>MEDIAN(E13,E14,E17)</f>
         <v>52.65</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="22">
         <f t="shared" si="2"/>
         <v>69.44</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="22">
         <f t="shared" si="2"/>
         <v>0.48549999999999999</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>0.68330000000000002</v>
-      </c>
-      <c r="I28" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>956</v>
-      </c>
-      <c r="J28" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>0.68689999999999996</v>
-      </c>
-      <c r="K28" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>961</v>
-      </c>
-      <c r="L28" s="24">
-        <f t="shared" si="2"/>
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="M28" s="24">
-        <f t="shared" si="2"/>
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="22">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>42.950499999999998</v>
       </c>
-      <c r="D29" s="24">
-        <f t="shared" ref="D29:M29" si="3">MEDIAN(D11,D12,D16)</f>
+      <c r="D29" s="22">
+        <f t="shared" ref="D29:K29" si="3">MEDIAN(D11,D12,D16)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="22">
         <f>MEDIAN(E11,E12,E16)</f>
         <v>52.65</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="22">
         <f t="shared" si="3"/>
         <v>69.540000000000006</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="22">
         <f t="shared" si="3"/>
         <v>0.48480000000000001</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>0.68759999999999999</v>
-      </c>
-      <c r="I29" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>962</v>
-      </c>
-      <c r="J29" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>0.6905</v>
-      </c>
-      <c r="K29" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>966</v>
-      </c>
-      <c r="L29" s="24">
-        <f t="shared" si="3"/>
-        <v>0.74980000000000002</v>
-      </c>
-      <c r="M29" s="24">
-        <f t="shared" si="3"/>
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="22">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>42.8215</v>
       </c>
-      <c r="D30" s="24">
-        <f t="shared" ref="D30:M30" si="4">MEDIAN(D9,D10,D15)</f>
+      <c r="D30" s="22">
+        <f t="shared" ref="D30:K30" si="4">MEDIAN(D9,D10,D15)</f>
         <v>33.44</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="22">
         <f t="shared" si="4"/>
         <v>52.64</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="22">
         <f t="shared" si="4"/>
         <v>69.569999999999993</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="22">
         <f t="shared" si="4"/>
         <v>0.48470000000000002</v>
       </c>
-      <c r="H30" s="24">
+      <c r="H30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>0.68479999999999996</v>
-      </c>
-      <c r="I30" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>958</v>
-      </c>
-      <c r="J30" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>0.68830000000000002</v>
-      </c>
-      <c r="K30" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>963</v>
-      </c>
-      <c r="L30" s="24">
-        <f t="shared" si="4"/>
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M30" s="24">
-        <f t="shared" si="4"/>
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="22">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>42.772199999999998</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="22">
         <f>MEDIAN(D10,D12,D14)</f>
         <v>33.44</v>
       </c>
-      <c r="E32" s="24">
-        <f t="shared" ref="E32:M32" si="5">MEDIAN(E10,E12,E14)</f>
+      <c r="E32" s="22">
+        <f t="shared" ref="E32:K32" si="5">MEDIAN(E10,E12,E14)</f>
         <v>52.65</v>
       </c>
-      <c r="F32" s="24">
+      <c r="F32" s="22">
         <f t="shared" si="5"/>
         <v>69.55</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="22">
         <f t="shared" si="5"/>
         <v>0.48549999999999999</v>
       </c>
-      <c r="H32" s="24">
+      <c r="H32" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>0.68479999999999996</v>
-      </c>
-      <c r="I32" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I32" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>958</v>
-      </c>
-      <c r="J32" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J32" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>0.68830000000000002</v>
-      </c>
-      <c r="K32" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K32" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>963</v>
-      </c>
-      <c r="L32" s="24">
-        <f t="shared" si="5"/>
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M32" s="24">
-        <f t="shared" si="5"/>
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" s="22">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>42.950499999999998</v>
       </c>
-      <c r="D33" s="24">
-        <f t="shared" ref="D33:M33" si="6">MEDIAN(D9,D11,D13)</f>
+      <c r="D33" s="22">
+        <f t="shared" ref="D33:K33" si="6">MEDIAN(D9,D11,D13)</f>
         <v>33.369999999999997</v>
       </c>
-      <c r="E33" s="24">
+      <c r="E33" s="22">
         <f t="shared" si="6"/>
         <v>52.65</v>
       </c>
-      <c r="F33" s="24">
+      <c r="F33" s="22">
         <f t="shared" si="6"/>
         <v>69.540000000000006</v>
       </c>
-      <c r="G33" s="24">
+      <c r="G33" s="22">
         <f t="shared" si="6"/>
         <v>0.48480000000000001</v>
       </c>
-      <c r="H33" s="24">
+      <c r="H33" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>0.68410000000000004</v>
-      </c>
-      <c r="I33" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I33" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>957</v>
-      </c>
-      <c r="J33" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J33" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>0.68759999999999999</v>
-      </c>
-      <c r="K33" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K33" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>962</v>
-      </c>
-      <c r="L33" s="24">
-        <f t="shared" si="6"/>
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M33" s="24">
-        <f t="shared" si="6"/>
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="22">
         <f>MEDIAN(C15:C17)</f>
         <v>42.8215</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="22">
         <f>MEDIAN(D15:D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E34" s="24">
-        <f t="shared" ref="E34:M34" si="7">MEDIAN(E15:E17)</f>
+      <c r="E34" s="22">
+        <f t="shared" ref="E34:K34" si="7">MEDIAN(E15:E17)</f>
         <v>52.6</v>
       </c>
-      <c r="F34" s="24">
+      <c r="F34" s="22">
         <f t="shared" si="7"/>
         <v>69.42</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34" s="22">
         <f t="shared" si="7"/>
         <v>0.48409999999999997</v>
       </c>
-      <c r="H34" s="24">
+      <c r="H34" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>0.6855</v>
-      </c>
-      <c r="I34" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I34" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>959</v>
-      </c>
-      <c r="J34" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J34" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>0.68910000000000005</v>
-      </c>
-      <c r="K34" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K34" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>964</v>
-      </c>
-      <c r="L34" s="24">
-        <f t="shared" si="7"/>
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="M34" s="24">
-        <f t="shared" si="7"/>
-        <v>1048</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="E19:K23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:M23"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2221,10 +1938,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2235,15 +1952,13 @@
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="6" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="17.77734375" customWidth="1"/>
     <col min="10" max="10" width="16.21875" customWidth="1"/>
     <col min="11" max="11" width="17.77734375" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2266,25 +1981,19 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2306,26 +2015,12 @@
       <c r="G2" s="7">
         <v>0.50900000000000001</v>
       </c>
-      <c r="H2" s="7">
-        <v>0.75480000000000003</v>
-      </c>
-      <c r="I2" s="7">
-        <v>1056</v>
-      </c>
-      <c r="J2" s="7">
-        <v>0.75839999999999996</v>
-      </c>
-      <c r="K2" s="7">
-        <v>1061</v>
-      </c>
-      <c r="L2" s="7">
-        <v>0.75839999999999996</v>
-      </c>
-      <c r="M2" s="7">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -2347,26 +2042,12 @@
       <c r="G3" s="8">
         <v>0.52349999999999997</v>
       </c>
-      <c r="H3" s="8">
-        <v>0.75409999999999999</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1055</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="K3" s="8">
-        <v>1059</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="M3" s="8">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -2388,26 +2069,12 @@
       <c r="G4" s="8">
         <v>0.52090000000000003</v>
       </c>
-      <c r="H4" s="8">
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1046</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="K4" s="8">
-        <v>1050</v>
-      </c>
-      <c r="L4" s="8">
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="M4" s="8">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2429,26 +2096,12 @@
       <c r="G5" s="8">
         <v>0.52569999999999995</v>
       </c>
-      <c r="H5" s="8">
-        <v>0.74480000000000002</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1042</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1046</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="M5" s="8">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -2458,38 +2111,24 @@
       <c r="C6" s="5">
         <v>43.224200000000003</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>33.56</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>53.02</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="23">
         <v>67.62</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="23">
         <v>0.52610000000000001</v>
       </c>
-      <c r="H6" s="25">
-        <v>0.73329999999999995</v>
-      </c>
-      <c r="I6" s="25">
-        <v>1026</v>
-      </c>
-      <c r="J6" s="25">
-        <v>0.73619999999999997</v>
-      </c>
-      <c r="K6" s="25">
-        <v>1030</v>
-      </c>
-      <c r="L6" s="25">
-        <v>0.73619999999999997</v>
-      </c>
-      <c r="M6" s="25">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2511,26 +2150,12 @@
       <c r="G7" s="11">
         <v>0.51370000000000005</v>
       </c>
-      <c r="H7" s="11">
-        <v>0.74839999999999995</v>
-      </c>
-      <c r="I7" s="11">
-        <v>1047</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="K7" s="11">
-        <v>1050</v>
-      </c>
-      <c r="L7" s="11">
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="M7" s="11">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>14</v>
       </c>
@@ -2552,31 +2177,17 @@
       <c r="G8" s="19">
         <v>0.52510000000000001</v>
       </c>
-      <c r="H8" s="19">
-        <v>0.74909999999999999</v>
-      </c>
-      <c r="I8" s="19">
-        <v>1048</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0.75129999999999997</v>
-      </c>
-      <c r="K8" s="19">
-        <v>1051</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0.75129999999999997</v>
-      </c>
-      <c r="M8" s="19">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>55</v>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>54</v>
       </c>
       <c r="C9" s="19">
         <v>43.620199999999997</v>
@@ -2593,31 +2204,17 @@
       <c r="G9" s="19">
         <v>0.51680000000000004</v>
       </c>
-      <c r="H9" s="26">
-        <v>0.74409999999999998</v>
-      </c>
-      <c r="I9" s="19">
-        <v>1041</v>
-      </c>
-      <c r="J9" s="19">
-        <v>0.74619999999999997</v>
-      </c>
-      <c r="K9" s="19">
-        <v>1044</v>
-      </c>
-      <c r="L9" s="19">
-        <v>0.74619999999999997</v>
-      </c>
-      <c r="M9" s="19">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>56</v>
+      <c r="H9" s="24"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>55</v>
       </c>
       <c r="C10" s="19">
         <v>43.218000000000004</v>
@@ -2634,320 +2231,208 @@
       <c r="G10" s="19">
         <v>0.52359999999999995</v>
       </c>
-      <c r="H10" s="19">
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="I10" s="19">
-        <v>1043</v>
-      </c>
-      <c r="J10" s="19">
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="K10" s="19">
-        <v>1046</v>
-      </c>
-      <c r="L10" s="19">
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="M10" s="19">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="24">
+        <v>43.872199999999999</v>
+      </c>
+      <c r="D11" s="24">
+        <v>34.24</v>
+      </c>
+      <c r="E11" s="24">
+        <v>53.31</v>
+      </c>
+      <c r="F11" s="24">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0.51749999999999996</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B12" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="24">
+        <v>43.644100000000002</v>
+      </c>
+      <c r="D12" s="24">
+        <v>33.97</v>
+      </c>
+      <c r="E12" s="24">
+        <v>53.13</v>
+      </c>
+      <c r="F12" s="24">
+        <v>68.290000000000006</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="24">
+        <v>43.685600000000001</v>
+      </c>
+      <c r="D13" s="24">
+        <v>33.840000000000003</v>
+      </c>
+      <c r="E13" s="24">
+        <v>53.06</v>
+      </c>
+      <c r="F13" s="24">
+        <v>68.3</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0.52</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="26">
-        <v>43.872199999999999</v>
-      </c>
-      <c r="D11" s="26">
-        <v>34.24</v>
-      </c>
-      <c r="E11" s="26">
-        <v>53.31</v>
-      </c>
-      <c r="F11" s="26">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="G11" s="26">
-        <v>0.51749999999999996</v>
-      </c>
-      <c r="H11" s="26">
-        <v>0.74409999999999998</v>
-      </c>
-      <c r="I11" s="26">
-        <v>1041</v>
-      </c>
-      <c r="J11" s="26">
-        <v>0.747</v>
-      </c>
-      <c r="K11" s="26">
-        <v>1045</v>
-      </c>
-      <c r="L11" s="26">
-        <v>0.747</v>
-      </c>
-      <c r="M11" s="26">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="26">
-        <v>43.644100000000002</v>
-      </c>
-      <c r="D12" s="26">
-        <v>33.97</v>
-      </c>
-      <c r="E12" s="26">
-        <v>53.13</v>
-      </c>
-      <c r="F12" s="26">
-        <v>68.290000000000006</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="H12" s="26">
-        <v>0.75129999999999997</v>
-      </c>
-      <c r="I12" s="26">
-        <v>1051</v>
-      </c>
-      <c r="J12" s="26">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="K12" s="26">
-        <v>1054</v>
-      </c>
-      <c r="L12" s="26">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="M12" s="26">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="26">
-        <v>43.685600000000001</v>
-      </c>
-      <c r="D13" s="26">
-        <v>33.840000000000003</v>
-      </c>
-      <c r="E13" s="26">
-        <v>53.06</v>
-      </c>
-      <c r="F13" s="26">
-        <v>68.3</v>
-      </c>
-      <c r="G13" s="26">
-        <v>0.52</v>
-      </c>
-      <c r="H13" s="26">
-        <v>0.74409999999999998</v>
-      </c>
-      <c r="I13" s="26">
-        <v>1041</v>
-      </c>
-      <c r="J13" s="26">
-        <v>0.747</v>
-      </c>
-      <c r="K13" s="26">
-        <v>1045</v>
-      </c>
-      <c r="L13" s="26">
-        <v>0.747</v>
-      </c>
-      <c r="M13" s="26">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="C14" s="24">
+        <v>43.317</v>
+      </c>
+      <c r="D14" s="24">
+        <v>34.03</v>
+      </c>
+      <c r="E14" s="24">
+        <v>53.24</v>
+      </c>
+      <c r="F14" s="24">
+        <v>68.33</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0.52349999999999997</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="26">
-        <v>43.317</v>
-      </c>
-      <c r="D14" s="26">
-        <v>34.03</v>
-      </c>
-      <c r="E14" s="26">
-        <v>53.24</v>
-      </c>
-      <c r="F14" s="26">
-        <v>68.33</v>
-      </c>
-      <c r="G14" s="26">
-        <v>0.52349999999999997</v>
-      </c>
-      <c r="H14" s="26">
-        <v>0.75549999999999995</v>
-      </c>
-      <c r="I14" s="26">
-        <v>1057</v>
-      </c>
-      <c r="J14" s="26">
-        <v>0.75839999999999996</v>
-      </c>
-      <c r="K14" s="26">
-        <v>1061</v>
-      </c>
-      <c r="L14" s="26">
-        <v>0.75839999999999996</v>
-      </c>
-      <c r="M14" s="26">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
+      <c r="B15" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="24">
+        <v>43.53</v>
+      </c>
+      <c r="D15" s="24">
+        <v>34.130000000000003</v>
+      </c>
+      <c r="E15" s="24">
+        <v>53.21</v>
+      </c>
+      <c r="F15" s="24">
+        <v>68.209999999999994</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0.52310000000000001</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="24">
+        <v>43.3065</v>
+      </c>
+      <c r="D16" s="24">
+        <v>33.65</v>
+      </c>
+      <c r="E16" s="24">
+        <v>53.02</v>
+      </c>
+      <c r="F16" s="24">
+        <v>67.819999999999993</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0.52210000000000001</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="26">
-        <v>43.53</v>
-      </c>
-      <c r="D15" s="26">
-        <v>34.130000000000003</v>
-      </c>
-      <c r="E15" s="26">
-        <v>53.21</v>
-      </c>
-      <c r="F15" s="26">
-        <v>68.209999999999994</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0.52310000000000001</v>
-      </c>
-      <c r="H15" s="26">
-        <v>0.74980000000000002</v>
-      </c>
-      <c r="I15" s="26">
-        <v>1049</v>
-      </c>
-      <c r="J15" s="26">
-        <v>0.75270000000000004</v>
-      </c>
-      <c r="K15" s="26">
-        <v>1053</v>
-      </c>
-      <c r="L15" s="26">
-        <v>0.75270000000000004</v>
-      </c>
-      <c r="M15" s="26">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="26">
-        <v>43.3065</v>
-      </c>
-      <c r="D16" s="26">
-        <v>33.65</v>
-      </c>
-      <c r="E16" s="26">
-        <v>53.02</v>
-      </c>
-      <c r="F16" s="26">
-        <v>67.819999999999993</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0.52210000000000001</v>
-      </c>
-      <c r="H16" s="26">
-        <v>0.74480000000000002</v>
-      </c>
-      <c r="I16" s="26">
-        <v>1042</v>
-      </c>
-      <c r="J16" s="26">
-        <v>0.747</v>
-      </c>
-      <c r="K16" s="26">
-        <v>1045</v>
-      </c>
-      <c r="L16" s="26">
-        <v>0.747</v>
-      </c>
-      <c r="M16" s="26">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="27">
+      <c r="B17" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="25">
         <v>43.733899999999998</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="25">
         <v>33.9</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="25">
         <v>53.23</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="25">
         <v>68.02</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="25">
         <v>0.52480000000000004</v>
       </c>
-      <c r="H17" s="27">
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="I17" s="27">
-        <v>1050</v>
-      </c>
-      <c r="J17" s="27">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="K17" s="27">
-        <v>1054</v>
-      </c>
-      <c r="L17" s="27">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="M17" s="27">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1">
@@ -2962,543 +2447,455 @@
       <c r="G18" s="1">
         <v>0.5131</v>
       </c>
-      <c r="H18" s="1">
-        <v>0.76480000000000004</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1070</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1073</v>
-      </c>
-      <c r="L18" s="1">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="M18" s="1">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="3">
         <v>35.5</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="3">
         <v>35.18</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="24">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="22">
         <f>MEDIAN(C7:C17)</f>
         <v>43.5535</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="22">
         <f>MEDIAN(D7:D17)</f>
         <v>33.86</v>
       </c>
-      <c r="E26" s="24">
-        <f t="shared" ref="E26:M26" si="0">MEDIAN(E7:E17)</f>
+      <c r="E26" s="22">
+        <f t="shared" ref="E26:K26" si="0">MEDIAN(E7:E17)</f>
         <v>53.12</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="22">
         <f t="shared" si="0"/>
         <v>68.290000000000006</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="22">
         <f t="shared" si="0"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>0.74839999999999995</v>
-      </c>
-      <c r="I26" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>1047</v>
-      </c>
-      <c r="J26" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="K26" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K26" s="22" t="e">
         <f t="shared" si="0"/>
-        <v>1050</v>
-      </c>
-      <c r="L26" s="24">
-        <f t="shared" si="0"/>
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="M26" s="24">
-        <f t="shared" si="0"/>
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="22">
         <f>MEDIAN(C9:C17)</f>
         <v>43.620199999999997</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="22">
         <f>MEDIAN(D9:D17)</f>
         <v>33.9</v>
       </c>
-      <c r="E27" s="24">
-        <f t="shared" ref="E27:M27" si="1">MEDIAN(E9:E17)</f>
+      <c r="E27" s="22">
+        <f t="shared" ref="E27:K27" si="1">MEDIAN(E9:E17)</f>
         <v>53.13</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="22">
         <f t="shared" si="1"/>
         <v>68.209999999999994</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="22">
         <f t="shared" si="1"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="I27" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>1043</v>
-      </c>
-      <c r="J27" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="K27" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K27" s="22" t="e">
         <f t="shared" si="1"/>
-        <v>1046</v>
-      </c>
-      <c r="L27" s="24">
-        <f t="shared" si="1"/>
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="M27" s="24">
-        <f t="shared" si="1"/>
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="22">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>43.685600000000001</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="22">
         <f>MEDIAN(D13,D14,D17)</f>
         <v>33.9</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="22">
         <f>MEDIAN(E13,E14,E17)</f>
         <v>53.23</v>
       </c>
-      <c r="F28" s="24">
-        <f t="shared" ref="F28:M28" si="2">MEDIAN(F13,F14,F17)</f>
+      <c r="F28" s="22">
+        <f t="shared" ref="F28:K28" si="2">MEDIAN(F13,F14,F17)</f>
         <v>68.3</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="22">
         <f t="shared" si="2"/>
         <v>0.52349999999999997</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="I28" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>1050</v>
-      </c>
-      <c r="J28" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="K28" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K28" s="22" t="e">
         <f t="shared" si="2"/>
-        <v>1054</v>
-      </c>
-      <c r="L28" s="24">
-        <f t="shared" si="2"/>
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="M28" s="24">
-        <f t="shared" si="2"/>
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="22">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>43.644100000000002</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="22">
         <f>MEDIAN(D11,D12,D16)</f>
         <v>33.97</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="22">
         <f>MEDIAN(E11,E12,E16)</f>
         <v>53.13</v>
       </c>
-      <c r="F29" s="24">
-        <f t="shared" ref="F29:M29" si="3">MEDIAN(F11,F12,F16)</f>
+      <c r="F29" s="22">
+        <f t="shared" ref="F29:K29" si="3">MEDIAN(F11,F12,F16)</f>
         <v>67.900000000000006</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="22">
         <f t="shared" si="3"/>
         <v>0.52210000000000001</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>0.74480000000000002</v>
-      </c>
-      <c r="I29" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>1042</v>
-      </c>
-      <c r="J29" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>0.747</v>
-      </c>
-      <c r="K29" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K29" s="22" t="e">
         <f t="shared" si="3"/>
-        <v>1045</v>
-      </c>
-      <c r="L29" s="24">
-        <f t="shared" si="3"/>
-        <v>0.747</v>
-      </c>
-      <c r="M29" s="24">
-        <f t="shared" si="3"/>
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="22">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>43.53</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="22">
         <f>MEDIAN(D9,D10,D15)</f>
         <v>33.85</v>
       </c>
-      <c r="E30" s="24">
-        <f t="shared" ref="E30:M30" si="4">MEDIAN(E9,E10,E15)</f>
+      <c r="E30" s="22">
+        <f t="shared" ref="E30:K30" si="4">MEDIAN(E9,E10,E15)</f>
         <v>53.06</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="22">
         <f t="shared" si="4"/>
         <v>68.209999999999994</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="22">
         <f t="shared" si="4"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H30" s="24">
+      <c r="H30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="I30" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>1043</v>
-      </c>
-      <c r="J30" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="K30" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K30" s="22" t="e">
         <f t="shared" si="4"/>
-        <v>1046</v>
-      </c>
-      <c r="L30" s="24">
-        <f t="shared" si="4"/>
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="M30" s="24">
-        <f t="shared" si="4"/>
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" s="22">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>43.317</v>
       </c>
-      <c r="D31" s="24">
-        <f t="shared" ref="D31:M31" si="5">MEDIAN(D10,D12,D14)</f>
+      <c r="D31" s="22">
+        <f t="shared" ref="D31:K31" si="5">MEDIAN(D10,D12,D14)</f>
         <v>33.97</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="22">
         <f t="shared" si="5"/>
         <v>53.13</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="22">
         <f t="shared" si="5"/>
         <v>68.290000000000006</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="22">
         <f t="shared" si="5"/>
         <v>0.52359999999999995</v>
       </c>
-      <c r="H31" s="24">
+      <c r="H31" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>0.75129999999999997</v>
-      </c>
-      <c r="I31" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I31" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>1051</v>
-      </c>
-      <c r="J31" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J31" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="K31" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K31" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>1054</v>
-      </c>
-      <c r="L31" s="24">
-        <f t="shared" si="5"/>
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="M31" s="24">
-        <f t="shared" si="5"/>
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="22">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>43.685600000000001</v>
       </c>
-      <c r="D32" s="24">
-        <f t="shared" ref="D32:M32" si="6">MEDIAN(D9,D11,D13)</f>
+      <c r="D32" s="22">
+        <f t="shared" ref="D32:K32" si="6">MEDIAN(D9,D11,D13)</f>
         <v>33.85</v>
       </c>
-      <c r="E32" s="24">
+      <c r="E32" s="22">
         <f t="shared" si="6"/>
         <v>53.06</v>
       </c>
-      <c r="F32" s="24">
+      <c r="F32" s="22">
         <f t="shared" si="6"/>
         <v>68.3</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="22">
         <f t="shared" si="6"/>
         <v>0.51749999999999996</v>
       </c>
-      <c r="H32" s="24">
+      <c r="H32" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>0.74409999999999998</v>
-      </c>
-      <c r="I32" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I32" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>1041</v>
-      </c>
-      <c r="J32" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J32" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>0.747</v>
-      </c>
-      <c r="K32" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K32" s="22" t="e">
         <f t="shared" si="6"/>
-        <v>1045</v>
-      </c>
-      <c r="L32" s="24">
-        <f t="shared" si="6"/>
-        <v>0.747</v>
-      </c>
-      <c r="M32" s="24">
-        <f t="shared" si="6"/>
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="24">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" s="22">
         <f>MEDIAN(C15:C17)</f>
         <v>43.53</v>
       </c>
-      <c r="D33" s="24">
-        <f t="shared" ref="D33:M33" si="7">MEDIAN(D15:D17)</f>
+      <c r="D33" s="22">
+        <f t="shared" ref="D33:K33" si="7">MEDIAN(D15:D17)</f>
         <v>33.9</v>
       </c>
-      <c r="E33" s="24">
+      <c r="E33" s="22">
         <f t="shared" si="7"/>
         <v>53.21</v>
       </c>
-      <c r="F33" s="24">
+      <c r="F33" s="22">
         <f t="shared" si="7"/>
         <v>68.02</v>
       </c>
-      <c r="G33" s="24">
+      <c r="G33" s="22">
         <f t="shared" si="7"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H33" s="24">
+      <c r="H33" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>0.74980000000000002</v>
-      </c>
-      <c r="I33" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="I33" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>1049</v>
-      </c>
-      <c r="J33" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="J33" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>0.75270000000000004</v>
-      </c>
-      <c r="K33" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="K33" s="22" t="e">
         <f t="shared" si="7"/>
-        <v>1053</v>
-      </c>
-      <c r="L33" s="24">
-        <f t="shared" si="7"/>
-        <v>0.75270000000000004</v>
-      </c>
-      <c r="M33" s="24">
-        <f t="shared" si="7"/>
-        <v>1053</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="E19:K23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:M23"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3906,7 +3303,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1">
@@ -3947,99 +3344,99 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="40"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="3">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="40"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="3">
         <v>35.5</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="46"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="3">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="46"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="3">
         <v>35.18</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="46"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="3">
         <v>31.63</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="50"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="49"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
@@ -4062,6 +3459,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -4290,38 +3704,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4344,9 +3730,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
rename adapt wce to freq wce
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Test Set Results.xlsx
+++ b/model_evaluations/Collated Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2670" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54BFFF4D-DDA8-47DA-B93D-860AA8415A1D}"/>
+  <xr:revisionPtr revIDLastSave="2719" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E289C948-D11D-404B-82C1-486A38BF1511}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Test Results" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="87">
   <si>
     <t>Validation BLEU</t>
   </si>
@@ -247,27 +247,12 @@
     <t>All-or-Nothing LSP FWCE</t>
   </si>
   <si>
-    <t>Median for FWCE</t>
-  </si>
-  <si>
-    <t>Median for All-or-Nothing FWCE</t>
-  </si>
-  <si>
-    <t>Median for Simple FWCE</t>
-  </si>
-  <si>
-    <t>Median for Fine-Banded FWCE</t>
-  </si>
-  <si>
     <t>Median for Unsampled FWCE</t>
   </si>
   <si>
     <t>Median for Intersected FWCE</t>
   </si>
   <si>
-    <t>Median for LSP FWCE</t>
-  </si>
-  <si>
     <t>Recall</t>
   </si>
   <si>
@@ -278,6 +263,42 @@
   </si>
   <si>
     <t>Annotated Concepts</t>
+  </si>
+  <si>
+    <t>Median for LSP WCE</t>
+  </si>
+  <si>
+    <t>Simple TFIDF WCE</t>
+  </si>
+  <si>
+    <t>All-or-Nothing Unsampled TFIDF WCE</t>
+  </si>
+  <si>
+    <t>Fine-Banded Unsampled TFIDF WCE</t>
+  </si>
+  <si>
+    <t>Simple Unsampled TFIDF WCE</t>
+  </si>
+  <si>
+    <t>Fine-Banded LSP WCE</t>
+  </si>
+  <si>
+    <t>Simple LSP WCE</t>
+  </si>
+  <si>
+    <t>All-or-Nothing LSP WCE</t>
+  </si>
+  <si>
+    <t>Median across all LSP WCE and FWCE methods</t>
+  </si>
+  <si>
+    <t>Median for All-or-Nothing WCE</t>
+  </si>
+  <si>
+    <t>Median for Simple WCE</t>
+  </si>
+  <si>
+    <t>Median for Fine-Banded WCE</t>
   </si>
 </sst>
 </file>
@@ -336,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -504,11 +525,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -628,6 +675,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -639,9 +689,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,6 +714,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -954,10 +1016,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8347FF-D187-4D6C-9C41-B96FB5C52911}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,16 +1059,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1466,7 +1528,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>49</v>
@@ -1501,7 +1563,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>50</v>
@@ -1536,7 +1598,7 @@
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>48</v>
@@ -1570,477 +1632,511 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C20" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D20" s="1">
         <v>37.71</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E20" s="1">
         <v>55.04</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F20" s="1">
         <v>66.48</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G20" s="1">
         <v>0.5131</v>
       </c>
-      <c r="H18" s="38"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="3">
-        <v>36.130000000000003</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="3">
-        <v>35.5</v>
-      </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+        <v>25</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="42"/>
       <c r="D21" s="3">
-        <v>35.409999999999997</v>
-      </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
+        <v>36.130000000000003</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+        <v>26</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="42"/>
       <c r="D22" s="3">
-        <v>35.18</v>
-      </c>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
+        <v>35.5</v>
+      </c>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="40"/>
+        <v>27</v>
+      </c>
+      <c r="B23" s="41"/>
       <c r="C23" s="42"/>
       <c r="D23" s="3">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="3">
+        <v>35.18</v>
+      </c>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="41"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="22">
+      <c r="B28" s="41"/>
+      <c r="C28" s="22">
         <f>MEDIAN(C7:C17)</f>
         <v>42.909500000000001</v>
       </c>
-      <c r="D26" s="22">
-        <f t="shared" ref="D26:K26" si="0">MEDIAN(D7:D17)</f>
+      <c r="D28" s="22">
+        <f t="shared" ref="D28:K28" si="0">MEDIAN(D7:D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E28" s="22">
         <f t="shared" si="0"/>
         <v>52.65</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F28" s="22">
         <f t="shared" si="0"/>
         <v>69.55</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G28" s="22">
         <f t="shared" si="0"/>
         <v>0.48509999999999998</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H28" s="22">
         <f t="shared" si="0"/>
         <v>1997</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I28" s="22">
         <f t="shared" si="0"/>
         <v>0.50619999999999998</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J28" s="22">
         <f t="shared" si="0"/>
         <v>0.57030000000000003</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K28" s="22">
         <f t="shared" si="0"/>
         <v>0.53659999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="22">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="22">
         <f>MEDIAN(C9:C17)</f>
         <v>42.887900000000002</v>
       </c>
-      <c r="D27" s="22">
-        <f t="shared" ref="D27:K27" si="1">MEDIAN(D9:D17)</f>
+      <c r="D29" s="22">
+        <f t="shared" ref="D29:K29" si="1">MEDIAN(D9:D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E29" s="22">
         <f t="shared" si="1"/>
         <v>52.65</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F29" s="22">
         <f t="shared" si="1"/>
         <v>69.540000000000006</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G29" s="22">
         <f t="shared" si="1"/>
         <v>0.48480000000000001</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H29" s="22">
         <f t="shared" si="1"/>
         <v>1992</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I29" s="22">
         <f t="shared" si="1"/>
         <v>0.50619999999999998</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J29" s="22">
         <f t="shared" si="1"/>
         <v>0.57030000000000003</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K29" s="22">
         <f t="shared" si="1"/>
         <v>0.53639999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="22">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="40"/>
+      <c r="C30" s="22">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>42.887900000000002</v>
       </c>
-      <c r="D28" s="22">
-        <f t="shared" ref="D28:K28" si="2">MEDIAN(D13,D14,D17)</f>
+      <c r="D30" s="22">
+        <f t="shared" ref="D30:K30" si="2">MEDIAN(D13,D14,D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E30" s="22">
         <f>MEDIAN(E13,E14,E17)</f>
         <v>52.65</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F30" s="22">
         <f t="shared" si="2"/>
         <v>69.44</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G30" s="22">
         <f t="shared" si="2"/>
         <v>0.48549999999999999</v>
       </c>
-      <c r="H28" s="22">
+      <c r="H30" s="22">
         <f t="shared" si="2"/>
         <v>1987</v>
       </c>
-      <c r="I28" s="22">
+      <c r="I30" s="22">
         <f t="shared" si="2"/>
         <v>0.50619999999999998</v>
       </c>
-      <c r="J28" s="22">
+      <c r="J30" s="22">
         <f t="shared" si="2"/>
         <v>0.57069999999999999</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K30" s="22">
         <f t="shared" si="2"/>
         <v>0.53639999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="22">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="40"/>
+      <c r="C31" s="22">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>42.950499999999998</v>
       </c>
-      <c r="D29" s="22">
-        <f t="shared" ref="D29:K29" si="3">MEDIAN(D11,D12,D16)</f>
+      <c r="D31" s="22">
+        <f t="shared" ref="D31:K31" si="3">MEDIAN(D11,D12,D16)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E31" s="22">
         <f>MEDIAN(E11,E12,E16)</f>
         <v>52.65</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F31" s="22">
         <f t="shared" si="3"/>
         <v>69.540000000000006</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G31" s="22">
         <f t="shared" si="3"/>
         <v>0.48480000000000001</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H31" s="22">
         <f t="shared" si="3"/>
         <v>1997</v>
       </c>
-      <c r="I29" s="22">
+      <c r="I31" s="22">
         <f t="shared" si="3"/>
         <v>0.50760000000000005</v>
       </c>
-      <c r="J29" s="22">
+      <c r="J31" s="22">
         <f t="shared" si="3"/>
         <v>0.56779999999999997</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K31" s="22">
         <f t="shared" si="3"/>
         <v>0.53600000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="22">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="40"/>
+      <c r="C32" s="22">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>42.8215</v>
       </c>
-      <c r="D30" s="22">
-        <f t="shared" ref="D30:K30" si="4">MEDIAN(D9,D10,D15)</f>
+      <c r="D32" s="22">
+        <f t="shared" ref="D32:K32" si="4">MEDIAN(D9,D10,D15)</f>
         <v>33.44</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E32" s="22">
         <f t="shared" si="4"/>
         <v>52.64</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F32" s="22">
         <f t="shared" si="4"/>
         <v>69.569999999999993</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G32" s="22">
         <f t="shared" si="4"/>
         <v>0.48470000000000002</v>
       </c>
-      <c r="H30" s="22">
+      <c r="H32" s="22">
         <f t="shared" si="4"/>
         <v>1992</v>
       </c>
-      <c r="I30" s="22">
+      <c r="I32" s="22">
         <f t="shared" si="4"/>
         <v>0.50449999999999995</v>
       </c>
-      <c r="J30" s="22">
+      <c r="J32" s="22">
         <f t="shared" si="4"/>
         <v>0.56789999999999996</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K32" s="22">
         <f t="shared" si="4"/>
         <v>0.53659999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="22">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="40"/>
+      <c r="C34" s="22">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>42.772199999999998</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D34" s="22">
         <f>MEDIAN(D10,D12,D14)</f>
         <v>33.44</v>
       </c>
-      <c r="E32" s="22">
-        <f t="shared" ref="E32:K32" si="5">MEDIAN(E10,E12,E14)</f>
+      <c r="E34" s="22">
+        <f t="shared" ref="E34:K34" si="5">MEDIAN(E10,E12,E14)</f>
         <v>52.65</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F34" s="22">
         <f t="shared" si="5"/>
         <v>69.55</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G34" s="22">
         <f t="shared" si="5"/>
         <v>0.48549999999999999</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H34" s="22">
         <f t="shared" si="5"/>
         <v>1987</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I34" s="22">
         <f t="shared" si="5"/>
         <v>0.50619999999999998</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J34" s="22">
         <f t="shared" si="5"/>
         <v>0.57169999999999999</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K34" s="22">
         <f t="shared" si="5"/>
         <v>0.53659999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="22">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="40"/>
+      <c r="C35" s="22">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>42.950499999999998</v>
       </c>
-      <c r="D33" s="22">
-        <f t="shared" ref="D33:K33" si="6">MEDIAN(D9,D11,D13)</f>
+      <c r="D35" s="22">
+        <f t="shared" ref="D35:K35" si="6">MEDIAN(D9,D11,D13)</f>
         <v>33.369999999999997</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E35" s="22">
         <f t="shared" si="6"/>
         <v>52.65</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F35" s="22">
         <f t="shared" si="6"/>
         <v>69.540000000000006</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G35" s="22">
         <f t="shared" si="6"/>
         <v>0.48480000000000001</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H35" s="22">
         <f t="shared" si="6"/>
         <v>1992</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I35" s="22">
         <f t="shared" si="6"/>
         <v>0.50619999999999998</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J35" s="22">
         <f t="shared" si="6"/>
         <v>0.57030000000000003</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K35" s="22">
         <f t="shared" si="6"/>
         <v>0.53639999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="44" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="22">
+      <c r="B36" s="40"/>
+      <c r="C36" s="22">
         <f>MEDIAN(C15:C17)</f>
         <v>42.8215</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D36" s="22">
         <f>MEDIAN(D15:D17)</f>
         <v>33.409999999999997</v>
       </c>
-      <c r="E34" s="22">
-        <f t="shared" ref="E34:K34" si="7">MEDIAN(E15:E17)</f>
+      <c r="E36" s="22">
+        <f t="shared" ref="E36:J36" si="7">MEDIAN(E15:E17)</f>
         <v>52.6</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F36" s="22">
         <f t="shared" si="7"/>
         <v>69.42</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G36" s="22">
         <f t="shared" si="7"/>
         <v>0.48409999999999997</v>
       </c>
-      <c r="H34" s="22">
+      <c r="H36" s="22">
         <f t="shared" si="7"/>
         <v>1997</v>
       </c>
-      <c r="I34" s="22">
+      <c r="I36" s="22">
         <f t="shared" si="7"/>
         <v>0.50529999999999997</v>
       </c>
-      <c r="J34" s="22">
+      <c r="J36" s="22">
         <f t="shared" si="7"/>
         <v>0.56789999999999996</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K36" s="22">
         <f>MEDIAN(K15:K17)</f>
         <v>0.53600000000000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="E21:K25"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:K23"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2050,10 +2146,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N31" sqref="N30:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2093,16 +2189,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2666,474 +2762,508 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+    </row>
+    <row r="20" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C20" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D20" s="1">
         <v>37.71</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E20" s="1">
         <v>55.04</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F20" s="1">
         <v>66.48</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G20" s="1">
         <v>0.5131</v>
       </c>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="3">
-        <v>36.130000000000003</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="3">
-        <v>35.5</v>
-      </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+        <v>25</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="42"/>
       <c r="D21" s="3">
-        <v>35.409999999999997</v>
-      </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
+        <v>36.130000000000003</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+        <v>26</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="42"/>
       <c r="D22" s="3">
-        <v>35.18</v>
-      </c>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
+        <v>35.5</v>
+      </c>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="40"/>
+        <v>27</v>
+      </c>
+      <c r="B23" s="41"/>
       <c r="C23" s="42"/>
       <c r="D23" s="3">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="3">
+        <v>35.18</v>
+      </c>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="41"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="3">
         <v>31.63</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="22">
+      <c r="B28" s="58"/>
+      <c r="C28" s="22">
         <f>MEDIAN(C7:C17)</f>
         <v>43.5535</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D28" s="22">
         <f>MEDIAN(D7:D17)</f>
         <v>33.86</v>
       </c>
-      <c r="E26" s="22">
-        <f t="shared" ref="E26:K26" si="0">MEDIAN(E7:E17)</f>
+      <c r="E28" s="22">
+        <f t="shared" ref="E28:K28" si="0">MEDIAN(E7:E17)</f>
         <v>53.12</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F28" s="22">
         <f t="shared" si="0"/>
         <v>68.290000000000006</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G28" s="22">
         <f t="shared" si="0"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H28" s="22">
         <f t="shared" si="0"/>
         <v>2184</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I28" s="22">
         <f t="shared" si="0"/>
         <v>0.55259999999999998</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J28" s="22">
         <f t="shared" si="0"/>
         <v>0.56579999999999997</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K28" s="22">
         <f t="shared" si="0"/>
         <v>0.55959999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="22">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="56"/>
+      <c r="C29" s="22">
         <f>MEDIAN(C9:C17)</f>
         <v>43.620199999999997</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D29" s="22">
         <f>MEDIAN(D9:D17)</f>
         <v>33.9</v>
       </c>
-      <c r="E27" s="22">
-        <f t="shared" ref="E27:K27" si="1">MEDIAN(E9:E17)</f>
+      <c r="E29" s="22">
+        <f t="shared" ref="E29:K29" si="1">MEDIAN(E9:E17)</f>
         <v>53.13</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F29" s="22">
         <f t="shared" si="1"/>
         <v>68.209999999999994</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G29" s="22">
         <f t="shared" si="1"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H29" s="22">
         <f t="shared" si="1"/>
         <v>2182</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I29" s="22">
         <f t="shared" si="1"/>
         <v>0.55259999999999998</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J29" s="22">
         <f t="shared" si="1"/>
         <v>0.56840000000000002</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K29" s="22">
         <f t="shared" si="1"/>
         <v>0.56030000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="22">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="56"/>
+      <c r="C30" s="22">
         <f>MEDIAN(C13,C14,C17)</f>
         <v>43.685600000000001</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D30" s="22">
         <f>MEDIAN(D13,D14,D17)</f>
         <v>33.9</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E30" s="22">
         <f>MEDIAN(E13,E14,E17)</f>
         <v>53.23</v>
       </c>
-      <c r="F28" s="22">
-        <f t="shared" ref="F28:K28" si="2">MEDIAN(F13,F14,F17)</f>
+      <c r="F30" s="22">
+        <f t="shared" ref="F30:K30" si="2">MEDIAN(F13,F14,F17)</f>
         <v>68.3</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G30" s="22">
         <f t="shared" si="2"/>
         <v>0.52349999999999997</v>
       </c>
-      <c r="H28" s="22">
+      <c r="H30" s="22">
         <f t="shared" si="2"/>
         <v>2182</v>
       </c>
-      <c r="I28" s="22">
+      <c r="I30" s="22">
         <f t="shared" si="2"/>
         <v>0.55259999999999998</v>
       </c>
-      <c r="J28" s="22">
+      <c r="J30" s="22">
         <f t="shared" si="2"/>
         <v>0.56369999999999998</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K30" s="22">
         <f t="shared" si="2"/>
         <v>0.56030000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="22">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="22">
         <f>MEDIAN(C11,C12,C16)</f>
         <v>43.644100000000002</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D31" s="22">
         <f>MEDIAN(D11,D12,D16)</f>
         <v>33.97</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E31" s="22">
         <f>MEDIAN(E11,E12,E16)</f>
         <v>53.13</v>
       </c>
-      <c r="F29" s="22">
-        <f t="shared" ref="F29:K29" si="3">MEDIAN(F11,F12,F16)</f>
+      <c r="F31" s="22">
+        <f t="shared" ref="F31:K31" si="3">MEDIAN(F11,F12,F16)</f>
         <v>67.900000000000006</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G31" s="22">
         <f t="shared" si="3"/>
         <v>0.52210000000000001</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H31" s="22">
         <f t="shared" si="3"/>
         <v>2171</v>
       </c>
-      <c r="I29" s="22">
+      <c r="I31" s="22">
         <f t="shared" si="3"/>
         <v>0.54990000000000006</v>
       </c>
-      <c r="J29" s="22">
+      <c r="J31" s="22">
         <f t="shared" si="3"/>
         <v>0.56840000000000002</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K31" s="22">
         <f t="shared" si="3"/>
         <v>0.55959999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="22">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="56"/>
+      <c r="C32" s="22">
         <f>MEDIAN(C9,C10,C15)</f>
         <v>43.53</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D32" s="22">
         <f>MEDIAN(D9,D10,D15)</f>
         <v>33.85</v>
       </c>
-      <c r="E30" s="22">
-        <f t="shared" ref="E30:K30" si="4">MEDIAN(E9,E10,E15)</f>
+      <c r="E32" s="22">
+        <f t="shared" ref="E32:K32" si="4">MEDIAN(E9,E10,E15)</f>
         <v>53.06</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F32" s="22">
         <f t="shared" si="4"/>
         <v>68.209999999999994</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G32" s="22">
         <f t="shared" si="4"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H30" s="22">
+      <c r="H32" s="22">
         <f t="shared" si="4"/>
         <v>2184</v>
       </c>
-      <c r="I30" s="22">
+      <c r="I32" s="22">
         <f t="shared" si="4"/>
         <v>0.55349999999999999</v>
       </c>
-      <c r="J30" s="22">
+      <c r="J32" s="22">
         <f t="shared" si="4"/>
         <v>0.5696</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K32" s="22">
         <f t="shared" si="4"/>
         <v>0.56189999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="22">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="56"/>
+      <c r="C33" s="22">
         <f>MEDIAN(C10,C12,C14)</f>
         <v>43.317</v>
       </c>
-      <c r="D31" s="22">
-        <f t="shared" ref="D31:K31" si="5">MEDIAN(D10,D12,D14)</f>
+      <c r="D33" s="22">
+        <f t="shared" ref="D33:K33" si="5">MEDIAN(D10,D12,D14)</f>
         <v>33.97</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E33" s="22">
         <f t="shared" si="5"/>
         <v>53.13</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F33" s="22">
         <f t="shared" si="5"/>
         <v>68.290000000000006</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G33" s="22">
         <f t="shared" si="5"/>
         <v>0.52359999999999995</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H33" s="22">
         <f t="shared" si="5"/>
         <v>2204</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I33" s="22">
         <f t="shared" si="5"/>
         <v>0.55569999999999997</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J33" s="22">
         <f t="shared" si="5"/>
         <v>0.56579999999999997</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K33" s="22">
         <f t="shared" si="5"/>
         <v>0.56069999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="22">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="56"/>
+      <c r="C34" s="22">
         <f>MEDIAN(C9,C11,C13)</f>
         <v>43.685600000000001</v>
       </c>
-      <c r="D32" s="22">
-        <f t="shared" ref="D32:K32" si="6">MEDIAN(D9,D11,D13)</f>
+      <c r="D34" s="22">
+        <f t="shared" ref="D34:K34" si="6">MEDIAN(D9,D11,D13)</f>
         <v>33.85</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E34" s="22">
         <f t="shared" si="6"/>
         <v>53.06</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F34" s="22">
         <f t="shared" si="6"/>
         <v>68.3</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G34" s="22">
         <f t="shared" si="6"/>
         <v>0.51749999999999996</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H34" s="22">
         <f t="shared" si="6"/>
         <v>2182</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I34" s="22">
         <f t="shared" si="6"/>
         <v>0.54990000000000006</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J34" s="22">
         <f t="shared" si="6"/>
         <v>0.56369999999999998</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K34" s="22">
         <f t="shared" si="6"/>
         <v>0.55679999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="44" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="22">
+      <c r="B35" s="56"/>
+      <c r="C35" s="22">
         <f>MEDIAN(C15:C17)</f>
         <v>43.53</v>
       </c>
-      <c r="D33" s="22">
-        <f t="shared" ref="D33:K33" si="7">MEDIAN(D15:D17)</f>
+      <c r="D35" s="22">
+        <f t="shared" ref="D35:K35" si="7">MEDIAN(D15:D17)</f>
         <v>33.9</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E35" s="22">
         <f t="shared" si="7"/>
         <v>53.21</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F35" s="22">
         <f t="shared" si="7"/>
         <v>68.02</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G35" s="22">
         <f t="shared" si="7"/>
         <v>0.52310000000000001</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H35" s="22">
         <f t="shared" si="7"/>
         <v>2171</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I35" s="22">
         <f t="shared" si="7"/>
         <v>0.55259999999999998</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J35" s="22">
         <f t="shared" si="7"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K35" s="22">
         <f t="shared" si="7"/>
         <v>0.56169999999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="E21:K25"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="E19:K23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
   </mergeCells>
@@ -3543,7 +3673,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="42" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1">
@@ -3584,7 +3714,7 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="3">
         <v>36.130000000000003</v>
       </c>
@@ -3604,10 +3734,10 @@
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="3">
         <v>35.5</v>
       </c>
@@ -3625,8 +3755,8 @@
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="3">
         <v>35.409999999999997</v>
       </c>
@@ -3644,8 +3774,8 @@
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="3">
         <v>35.18</v>
       </c>
@@ -3663,8 +3793,8 @@
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="42"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="3">
         <v>31.63</v>
       </c>
@@ -3699,6 +3829,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -3927,38 +4074,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3981,9 +4100,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>